<commit_message>
Coste estimado equipamiento coche
</commit_message>
<xml_diff>
--- a/Coste_Proyecto.xlsx
+++ b/Coste_Proyecto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\batiste\Documents\Universidad\césure\Uniraid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\batiste\Documents\Universidad\césure\Uniraid\UniR20 JS-BV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEDE6D3-47AC-4BB8-9937-C7EBCADCB4F6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B91A328-C172-4BCE-BB57-34CDB7F7A341}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="7" xr2:uid="{0252D24D-8C4E-46DC-8752-B88423AA2B2C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0252D24D-8C4E-46DC-8752-B88423AA2B2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Coste TOTAL" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="79">
   <si>
     <t>Item</t>
   </si>
@@ -56,6 +56,219 @@
   </si>
   <si>
     <t>Pre-inscripción</t>
+  </si>
+  <si>
+    <t>A pagar antes del 30 de junio 2019. Plaza asegurada para UniRaid</t>
+  </si>
+  <si>
+    <t>Inscripción</t>
+  </si>
+  <si>
+    <t>Antes del 23 de Enero del 2020</t>
+  </si>
+  <si>
+    <t>Coche</t>
+  </si>
+  <si>
+    <t>Peugeot 205 o Peugeot 206</t>
+  </si>
+  <si>
+    <t>ITV+ Impuestos</t>
+  </si>
+  <si>
+    <t>A verificar</t>
+  </si>
+  <si>
+    <t>Aseguradora</t>
+  </si>
+  <si>
+    <t>Puesta a punto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A verificar (Posibilidad de hacerlo nosotros mismos) </t>
+  </si>
+  <si>
+    <t>Nosotros en el coche?? En un remolque??</t>
+  </si>
+  <si>
+    <t>Equipamiento coche</t>
+  </si>
+  <si>
+    <t>A verificar (carta verde, pasaportes)</t>
+  </si>
+  <si>
+    <t>Gasolina</t>
+  </si>
+  <si>
+    <t>Manutención</t>
+  </si>
+  <si>
+    <t>Comidas a medio dia, etc</t>
+  </si>
+  <si>
+    <t>A calcular</t>
+  </si>
+  <si>
+    <t>Marca</t>
+  </si>
+  <si>
+    <t>Modelo</t>
+  </si>
+  <si>
+    <t>Precio</t>
+  </si>
+  <si>
+    <t>Origen</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Contacto</t>
+  </si>
+  <si>
+    <t>Peugeot</t>
+  </si>
+  <si>
+    <t>Huesca</t>
+  </si>
+  <si>
+    <t> en perfecto estado, tanto de mecánica como de chapa. La itv recen pasada, se vende por no emplear, duerme siempre en el garaje. Color Marron</t>
+  </si>
+  <si>
+    <t>Año</t>
+  </si>
+  <si>
+    <t>Kms</t>
+  </si>
+  <si>
+    <t>Beni 648241164</t>
+  </si>
+  <si>
+    <t>205 1.2 60 CV</t>
+  </si>
+  <si>
+    <t>205 SR 65 CV</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>Modelo basico y sencillo irrompible. Pocos km y unico dueño. Itv hasta agosto de 2019 ruedas nuevas tapiceria en buen estado. </t>
+  </si>
+  <si>
+    <t>Salazar Car 610973036</t>
+  </si>
+  <si>
+    <t>Huelva</t>
+  </si>
+  <si>
+    <t>205 1.1 57 CV</t>
+  </si>
+  <si>
+    <t>Coste Total</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Transporte</t>
+  </si>
+  <si>
+    <t>Coste TOTAL</t>
+  </si>
+  <si>
+    <t>Proyecto Solidario</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Extintor de mano</t>
+  </si>
+  <si>
+    <t>Triangulos</t>
+  </si>
+  <si>
+    <t>Chalecos reflectantes</t>
+  </si>
+  <si>
+    <t>Cinta para desatascar(eslinga)</t>
+  </si>
+  <si>
+    <t>Grilletes</t>
+  </si>
+  <si>
+    <t>Botiquín</t>
+  </si>
+  <si>
+    <t>Bomba de inchado manual</t>
+  </si>
+  <si>
+    <t>Sacos de dormir</t>
+  </si>
+  <si>
+    <t>Bidón de combustible 20L</t>
+  </si>
+  <si>
+    <t>Tienda de campaña</t>
+  </si>
+  <si>
+    <t>Movil GPS</t>
+  </si>
+  <si>
+    <t>Brújula</t>
+  </si>
+  <si>
+    <t>Luz frontal</t>
+  </si>
+  <si>
+    <t>Mapa de Marruecos</t>
+  </si>
+  <si>
+    <t>Belcros</t>
+  </si>
+  <si>
+    <t>2ª rueda de recambio</t>
+  </si>
+  <si>
+    <t>Caja de herramientas</t>
+  </si>
+  <si>
+    <t>Rampas de desatasco</t>
+  </si>
+  <si>
+    <t>No obligatorio</t>
+  </si>
+  <si>
+    <t>Gafas tormenta de arena</t>
+  </si>
+  <si>
+    <t>Pala</t>
+  </si>
+  <si>
+    <t>Filtro combustible</t>
+  </si>
+  <si>
+    <t>Filtro aire</t>
+  </si>
+  <si>
+    <t>Walki</t>
+  </si>
+  <si>
+    <t>Toma mechero</t>
+  </si>
+  <si>
+    <t>Anclajes</t>
+  </si>
+  <si>
+    <t>bestek</t>
+  </si>
+  <si>
+    <t>Total estimado</t>
+  </si>
+  <si>
+    <t>Total real</t>
   </si>
   <si>
     <r>
@@ -78,218 +291,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>)</t>
+      <t>)estimado Maika</t>
     </r>
   </si>
   <si>
-    <t>A pagar antes del 30 de junio 2019. Plaza asegurada para UniRaid</t>
-  </si>
-  <si>
-    <t>Inscripción</t>
-  </si>
-  <si>
-    <t>Antes del 23 de Enero del 2020</t>
-  </si>
-  <si>
-    <t>Coche</t>
-  </si>
-  <si>
-    <t>Peugeot 205 o Peugeot 206</t>
-  </si>
-  <si>
-    <t>ITV+ Impuestos</t>
-  </si>
-  <si>
-    <t>A verificar</t>
-  </si>
-  <si>
-    <t>Aseguradora</t>
-  </si>
-  <si>
-    <t>Puesta a punto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A verificar (Posibilidad de hacerlo nosotros mismos) </t>
-  </si>
-  <si>
-    <t>Nosotros en el coche?? En un remolque??</t>
-  </si>
-  <si>
-    <t>Equipamiento coche</t>
-  </si>
-  <si>
-    <t>A verificar (carta verde, pasaportes)</t>
-  </si>
-  <si>
-    <t>Gasolina</t>
-  </si>
-  <si>
-    <t>Manutención</t>
-  </si>
-  <si>
-    <t>Comidas a medio dia, etc</t>
-  </si>
-  <si>
-    <t>A calcular</t>
-  </si>
-  <si>
-    <t>Marca</t>
-  </si>
-  <si>
-    <t>Modelo</t>
-  </si>
-  <si>
-    <t>Precio</t>
-  </si>
-  <si>
-    <t>Origen</t>
-  </si>
-  <si>
-    <t>Estado</t>
-  </si>
-  <si>
-    <t>Contacto</t>
-  </si>
-  <si>
-    <t>Peugeot</t>
-  </si>
-  <si>
-    <t>Huesca</t>
-  </si>
-  <si>
-    <t> en perfecto estado, tanto de mecánica como de chapa. La itv recen pasada, se vende por no emplear, duerme siempre en el garaje. Color Marron</t>
-  </si>
-  <si>
-    <t>Año</t>
-  </si>
-  <si>
-    <t>Kms</t>
-  </si>
-  <si>
-    <t>Beni 648241164</t>
-  </si>
-  <si>
-    <t>205 1.2 60 CV</t>
-  </si>
-  <si>
-    <t>205 SR 65 CV</t>
-  </si>
-  <si>
-    <t>Madrid</t>
-  </si>
-  <si>
-    <t>Modelo basico y sencillo irrompible. Pocos km y unico dueño. Itv hasta agosto de 2019 ruedas nuevas tapiceria en buen estado. </t>
-  </si>
-  <si>
-    <t>Salazar Car 610973036</t>
-  </si>
-  <si>
-    <t>Huelva</t>
-  </si>
-  <si>
-    <t>205 1.1 57 CV</t>
-  </si>
-  <si>
-    <t>Coste Total</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>Transporte</t>
-  </si>
-  <si>
-    <t>Coste TOTAL</t>
-  </si>
-  <si>
-    <t>Proyecto Solidario</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Observaciones</t>
-  </si>
-  <si>
-    <t>Extintor de mano</t>
-  </si>
-  <si>
-    <t>Triangulos</t>
-  </si>
-  <si>
-    <t>Chalecos reflectantes</t>
-  </si>
-  <si>
-    <t>Cinta para desatascar(eslinga)</t>
-  </si>
-  <si>
-    <t>Grilletes</t>
-  </si>
-  <si>
-    <t>Botiquín</t>
-  </si>
-  <si>
-    <t>Bomba de inchado manual</t>
-  </si>
-  <si>
-    <t>Sacos de dormir</t>
-  </si>
-  <si>
-    <t>Bidón de combustible 20L</t>
-  </si>
-  <si>
-    <t>Tienda de campaña</t>
-  </si>
-  <si>
-    <t>Movil GPS</t>
-  </si>
-  <si>
-    <t>Brújula</t>
-  </si>
-  <si>
-    <t>Luz frontal</t>
-  </si>
-  <si>
-    <t>Mapa de Marruecos</t>
-  </si>
-  <si>
-    <t>Belcros</t>
-  </si>
-  <si>
-    <t>2ª rueda de recambio</t>
-  </si>
-  <si>
-    <t>Caja de herramientas</t>
-  </si>
-  <si>
-    <t>Rampas de desatasco</t>
-  </si>
-  <si>
-    <t>No obligatorio</t>
-  </si>
-  <si>
-    <t>Gafas tormenta de arena</t>
-  </si>
-  <si>
-    <t>Pala</t>
-  </si>
-  <si>
-    <t>Filtro combustible</t>
-  </si>
-  <si>
-    <t>Filtro aire</t>
-  </si>
-  <si>
-    <t>Walki</t>
-  </si>
-  <si>
-    <t>Toma mechero</t>
-  </si>
-  <si>
-    <t>Con varios Usbs, y otros enchufes tipo mechero(obligado por reglamento)</t>
-  </si>
-  <si>
-    <t>2 o 3</t>
+    <t>TOTAL Estimado Batiste</t>
+  </si>
+  <si>
+    <t>TOTAL real</t>
   </si>
 </sst>
 </file>
@@ -347,7 +356,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -564,12 +573,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -585,12 +644,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -599,7 +652,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -915,19 +977,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2BFAF8A-A11B-4F7B-8DDC-92AA48C4A0E8}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="43.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -935,13 +998,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -949,147 +1018,179 @@
       <c r="C2" s="2">
         <v>400</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>7</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2">
         <f>1890-C2</f>
         <v>1490</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2">
         <v>600</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>11</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2">
         <v>100</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2">
         <v>150</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2">
         <v>1000</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2">
         <v>100</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2">
         <v>150</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2">
         <v>300</v>
       </c>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="22">
+        <f>'Equipamiento Coche'!C28</f>
+        <v>1246</v>
+      </c>
+      <c r="E10" s="22">
+        <f>'Equipamiento Coche'!D28</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2">
         <v>300</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2">
         <v>150</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15">
+      <c r="B14" s="20"/>
+      <c r="C14" s="13">
         <f>SUM(C2:C12)</f>
         <v>4740</v>
       </c>
-      <c r="D14" s="12"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1122,7 +1223,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1143,7 +1244,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1158,7 +1259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B91F7E-FBAD-46C7-A681-762405B44D88}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1168,53 +1269,53 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
       <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
         <v>32</v>
-      </c>
-      <c r="H2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3">
         <v>500</v>
       </c>
       <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>31</v>
-      </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G3">
         <v>1988</v>
@@ -1225,22 +1326,22 @@
     </row>
     <row r="4" spans="1:8" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4">
         <v>500</v>
       </c>
       <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="F4" t="s">
         <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
       </c>
       <c r="G4">
         <v>1995</v>
@@ -1251,16 +1352,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>399</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5">
         <v>665191138</v>
@@ -1290,7 +1391,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1311,7 +1412,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1326,13 +1427,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0061F2D-3EFE-4AA8-8C50-DBC1B8D7262C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1353,7 +1456,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1374,7 +1477,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1387,24 +1490,24 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E84D5B8-BDE6-40AC-88AB-28FD121D3B6F}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="4" max="4" width="67" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1412,269 +1515,383 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="2">
+        <f>90*B3</f>
+        <v>180</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2">
+        <f>12*B4</f>
+        <v>24</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="2">
+        <f>6*B5</f>
+        <v>12</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="2">
         <v>2</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <f>15*B8</f>
+        <v>30</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B9" s="2">
         <v>2</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <f>50*2</f>
+        <v>100</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2">
+        <f>140*2</f>
+        <v>280</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <v>50</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <v>45</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B14" s="2">
         <v>2</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <f>16*2</f>
+        <v>32</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2">
+        <f>12*B16</f>
+        <v>24</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="2">
         <v>1</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <f>9*1</f>
+        <v>9</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <v>100</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B20" s="2">
-        <v>2</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2">
+        <v>50</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B21" s="2">
         <v>2</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <v>100</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B22" s="2">
         <v>2</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="8" t="s">
+      <c r="C22" s="2">
+        <f>15*2</f>
+        <v>30</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>70</v>
-      </c>
       <c r="B23" s="2">
-        <v>1</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>25</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B24" s="2">
         <v>1</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <v>25</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2">
+        <v>12</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <v>29</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2">
+        <v>25</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="8"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" s="11">
-        <v>1</v>
-      </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="12" t="s">
-        <v>74</v>
-      </c>
+      <c r="B28" s="11">
+        <f>SUM(B3:B27)</f>
+        <v>38</v>
+      </c>
+      <c r="C28" s="11">
+        <f>SUM(C3:C27)</f>
+        <v>1246</v>
+      </c>
+      <c r="D28" s="11">
+        <f>SUM(D3:D27)</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1694,7 +1911,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>